<commit_message>
Pequeños cambios banco contenidos (escaleta)
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado07/guion07/Escaleta CN_07_07_CO.xlsx
+++ b/fuentes/contenidos/grado07/guion07/Escaleta CN_07_07_CO.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\German\Documents\Aulaplaneta All\Trabajos de editor\EDITOR\ESCALETAS\Escaletas  grupo  3\CN_07_07_CO\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\German\Documents\GitHub\CienciasNaturales\fuentes\contenidos\grado07\guion07\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -756,7 +756,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -765,14 +765,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -810,13 +802,6 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="12"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -950,20 +935,20 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="99">
+  <cellXfs count="97">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -971,27 +956,27 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1007,12 +992,53 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1022,108 +1048,19 @@
     <xf numFmtId="0" fontId="4" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="12" borderId="1" xfId="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="1" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1137,7 +1074,7 @@
     <xf numFmtId="0" fontId="1" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1150,6 +1087,48 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1459,8 +1438,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U298"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="L46" sqref="L46"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="L52" sqref="L52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1489,94 +1468,94 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" s="9" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="78" t="s">
+      <c r="A1" s="85" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="80" t="s">
+      <c r="B1" s="87" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="82" t="s">
+      <c r="C1" s="89" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="78" t="s">
+      <c r="D1" s="85" t="s">
         <v>111</v>
       </c>
-      <c r="E1" s="80" t="s">
+      <c r="E1" s="87" t="s">
         <v>112</v>
       </c>
-      <c r="F1" s="84" t="s">
+      <c r="F1" s="91" t="s">
         <v>113</v>
       </c>
-      <c r="G1" s="76" t="s">
+      <c r="G1" s="83" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="84" t="s">
+      <c r="H1" s="91" t="s">
         <v>114</v>
       </c>
-      <c r="I1" s="84" t="s">
+      <c r="I1" s="91" t="s">
         <v>108</v>
       </c>
-      <c r="J1" s="86" t="s">
+      <c r="J1" s="93" t="s">
         <v>4</v>
       </c>
-      <c r="K1" s="88" t="s">
+      <c r="K1" s="95" t="s">
         <v>109</v>
       </c>
-      <c r="L1" s="76" t="s">
+      <c r="L1" s="83" t="s">
         <v>14</v>
       </c>
-      <c r="M1" s="94" t="s">
+      <c r="M1" s="78" t="s">
         <v>21</v>
       </c>
-      <c r="N1" s="94"/>
-      <c r="O1" s="95" t="s">
+      <c r="N1" s="78"/>
+      <c r="O1" s="79" t="s">
         <v>110</v>
       </c>
-      <c r="P1" s="95" t="s">
+      <c r="P1" s="79" t="s">
         <v>115</v>
       </c>
-      <c r="Q1" s="92" t="s">
+      <c r="Q1" s="76" t="s">
         <v>86</v>
       </c>
-      <c r="R1" s="97" t="s">
+      <c r="R1" s="81" t="s">
         <v>87</v>
       </c>
-      <c r="S1" s="92" t="s">
+      <c r="S1" s="76" t="s">
         <v>88</v>
       </c>
-      <c r="T1" s="90" t="s">
+      <c r="T1" s="74" t="s">
         <v>89</v>
       </c>
-      <c r="U1" s="92" t="s">
+      <c r="U1" s="76" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="2" spans="1:21" s="9" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="79"/>
-      <c r="B2" s="81"/>
-      <c r="C2" s="83"/>
-      <c r="D2" s="79"/>
-      <c r="E2" s="81"/>
-      <c r="F2" s="85"/>
-      <c r="G2" s="77"/>
-      <c r="H2" s="85"/>
-      <c r="I2" s="85"/>
-      <c r="J2" s="87"/>
-      <c r="K2" s="89"/>
-      <c r="L2" s="77"/>
+      <c r="A2" s="86"/>
+      <c r="B2" s="88"/>
+      <c r="C2" s="90"/>
+      <c r="D2" s="86"/>
+      <c r="E2" s="88"/>
+      <c r="F2" s="92"/>
+      <c r="G2" s="84"/>
+      <c r="H2" s="92"/>
+      <c r="I2" s="92"/>
+      <c r="J2" s="94"/>
+      <c r="K2" s="96"/>
+      <c r="L2" s="84"/>
       <c r="M2" s="10" t="s">
         <v>91</v>
       </c>
       <c r="N2" s="10" t="s">
         <v>92</v>
       </c>
-      <c r="O2" s="96"/>
-      <c r="P2" s="96"/>
-      <c r="Q2" s="93"/>
-      <c r="R2" s="98"/>
-      <c r="S2" s="93"/>
-      <c r="T2" s="91"/>
-      <c r="U2" s="93"/>
+      <c r="O2" s="80"/>
+      <c r="P2" s="80"/>
+      <c r="Q2" s="77"/>
+      <c r="R2" s="82"/>
+      <c r="S2" s="77"/>
+      <c r="T2" s="75"/>
+      <c r="U2" s="77"/>
     </row>
     <row r="3" spans="1:21" s="35" customFormat="1" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A3" s="11" t="s">
@@ -1592,7 +1571,7 @@
         <v>124</v>
       </c>
       <c r="E3" s="6"/>
-      <c r="F3" s="73"/>
+      <c r="F3" s="72"/>
       <c r="G3" s="38"/>
       <c r="H3" s="25"/>
       <c r="I3" s="16"/>
@@ -1603,11 +1582,11 @@
       <c r="N3" s="20"/>
       <c r="O3" s="8"/>
       <c r="P3" s="25"/>
-      <c r="Q3" s="70"/>
-      <c r="R3" s="71"/>
-      <c r="S3" s="70"/>
-      <c r="T3" s="72"/>
-      <c r="U3" s="70"/>
+      <c r="Q3" s="69"/>
+      <c r="R3" s="70"/>
+      <c r="S3" s="69"/>
+      <c r="T3" s="71"/>
+      <c r="U3" s="69"/>
     </row>
     <row r="4" spans="1:21" s="35" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="11" t="s">
@@ -1625,7 +1604,7 @@
       <c r="E4" s="6" t="s">
         <v>125</v>
       </c>
-      <c r="F4" s="73"/>
+      <c r="F4" s="72"/>
       <c r="G4" s="38"/>
       <c r="H4" s="25"/>
       <c r="I4" s="16"/>
@@ -1636,11 +1615,11 @@
       <c r="N4" s="20"/>
       <c r="O4" s="8"/>
       <c r="P4" s="25"/>
-      <c r="Q4" s="70"/>
-      <c r="R4" s="71"/>
-      <c r="S4" s="70"/>
-      <c r="T4" s="72"/>
-      <c r="U4" s="70"/>
+      <c r="Q4" s="69"/>
+      <c r="R4" s="70"/>
+      <c r="S4" s="69"/>
+      <c r="T4" s="71"/>
+      <c r="U4" s="69"/>
     </row>
     <row r="5" spans="1:21" s="35" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="11" t="s">
@@ -1658,7 +1637,7 @@
       <c r="E5" s="6" t="s">
         <v>125</v>
       </c>
-      <c r="F5" s="75" t="s">
+      <c r="F5" s="73" t="s">
         <v>220</v>
       </c>
       <c r="G5" s="38" t="s">
@@ -1687,19 +1666,19 @@
       <c r="P5" s="25" t="s">
         <v>19</v>
       </c>
-      <c r="Q5" s="70">
+      <c r="Q5" s="69">
         <v>6</v>
       </c>
-      <c r="R5" s="71" t="s">
+      <c r="R5" s="70" t="s">
         <v>194</v>
       </c>
-      <c r="S5" s="70" t="s">
+      <c r="S5" s="69" t="s">
         <v>195</v>
       </c>
-      <c r="T5" s="72" t="s">
+      <c r="T5" s="71" t="s">
         <v>199</v>
       </c>
-      <c r="U5" s="70" t="s">
+      <c r="U5" s="69" t="s">
         <v>196</v>
       </c>
     </row>
@@ -2179,7 +2158,7 @@
         <v>120</v>
       </c>
       <c r="O16" s="8"/>
-      <c r="P16" s="69" t="s">
+      <c r="P16" s="25" t="s">
         <v>20</v>
       </c>
       <c r="Q16" s="64">
@@ -2243,19 +2222,19 @@
       <c r="P17" s="25" t="s">
         <v>19</v>
       </c>
-      <c r="Q17" s="70">
+      <c r="Q17" s="69">
         <v>6</v>
       </c>
-      <c r="R17" s="71" t="s">
+      <c r="R17" s="70" t="s">
         <v>194</v>
       </c>
-      <c r="S17" s="70" t="s">
+      <c r="S17" s="69" t="s">
         <v>195</v>
       </c>
-      <c r="T17" s="72" t="s">
+      <c r="T17" s="71" t="s">
         <v>200</v>
       </c>
-      <c r="U17" s="70" t="s">
+      <c r="U17" s="69" t="s">
         <v>196</v>
       </c>
     </row>
@@ -2496,11 +2475,11 @@
       <c r="N22" s="63"/>
       <c r="O22" s="57"/>
       <c r="P22" s="25"/>
-      <c r="Q22" s="70"/>
-      <c r="R22" s="71"/>
-      <c r="S22" s="70"/>
-      <c r="T22" s="72"/>
-      <c r="U22" s="70"/>
+      <c r="Q22" s="69"/>
+      <c r="R22" s="70"/>
+      <c r="S22" s="69"/>
+      <c r="T22" s="71"/>
+      <c r="U22" s="69"/>
     </row>
     <row r="23" spans="1:21" s="67" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A23" s="53" t="s">
@@ -2547,19 +2526,19 @@
       <c r="P23" s="25" t="s">
         <v>19</v>
       </c>
-      <c r="Q23" s="70">
+      <c r="Q23" s="69">
         <v>6</v>
       </c>
-      <c r="R23" s="71" t="s">
+      <c r="R23" s="70" t="s">
         <v>194</v>
       </c>
-      <c r="S23" s="70" t="s">
+      <c r="S23" s="69" t="s">
         <v>195</v>
       </c>
-      <c r="T23" s="72" t="s">
+      <c r="T23" s="71" t="s">
         <v>201</v>
       </c>
-      <c r="U23" s="70" t="s">
+      <c r="U23" s="69" t="s">
         <v>196</v>
       </c>
     </row>
@@ -2892,7 +2871,7 @@
         <v>121</v>
       </c>
       <c r="O31" s="8"/>
-      <c r="P31" s="69" t="s">
+      <c r="P31" s="25" t="s">
         <v>20</v>
       </c>
       <c r="Q31" s="64">
@@ -2937,7 +2916,7 @@
       <c r="M32" s="20"/>
       <c r="N32" s="20"/>
       <c r="O32" s="8"/>
-      <c r="P32" s="69"/>
+      <c r="P32" s="25"/>
       <c r="Q32" s="64"/>
       <c r="R32" s="65"/>
       <c r="S32" s="64"/>
@@ -3150,7 +3129,7 @@
         <v>36</v>
       </c>
       <c r="O37" s="8"/>
-      <c r="P37" s="69" t="s">
+      <c r="P37" s="25" t="s">
         <v>20</v>
       </c>
       <c r="Q37" s="64">
@@ -3333,7 +3312,7 @@
         <v>32</v>
       </c>
       <c r="O40" s="57"/>
-      <c r="P40" s="74" t="s">
+      <c r="P40" s="59" t="s">
         <v>20</v>
       </c>
       <c r="Q40" s="64">
@@ -3506,7 +3485,7 @@
       </c>
       <c r="N43" s="20"/>
       <c r="O43" s="8"/>
-      <c r="P43" s="69" t="s">
+      <c r="P43" s="25" t="s">
         <v>20</v>
       </c>
       <c r="Q43" s="64">
@@ -3721,7 +3700,7 @@
       </c>
       <c r="O47" s="8"/>
       <c r="P47" s="25" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="Q47" s="64">
         <v>6</v>
@@ -4953,14 +4932,6 @@
     <row r="298" hidden="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="T1:T2"/>
-    <mergeCell ref="U1:U2"/>
-    <mergeCell ref="M1:N1"/>
-    <mergeCell ref="O1:O2"/>
-    <mergeCell ref="P1:P2"/>
-    <mergeCell ref="Q1:Q2"/>
-    <mergeCell ref="R1:R2"/>
-    <mergeCell ref="S1:S2"/>
     <mergeCell ref="L1:L2"/>
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="B1:B2"/>
@@ -4973,6 +4944,14 @@
     <mergeCell ref="I1:I2"/>
     <mergeCell ref="J1:J2"/>
     <mergeCell ref="K1:K2"/>
+    <mergeCell ref="T1:T2"/>
+    <mergeCell ref="U1:U2"/>
+    <mergeCell ref="M1:N1"/>
+    <mergeCell ref="O1:O2"/>
+    <mergeCell ref="P1:P2"/>
+    <mergeCell ref="Q1:Q2"/>
+    <mergeCell ref="R1:R2"/>
+    <mergeCell ref="S1:S2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Guion revisado editor y solicitud gráfica
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado07/guion07/Escaleta CN_07_07_CO.xlsx
+++ b/fuentes/contenidos/grado07/guion07/Escaleta CN_07_07_CO.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\German\Documents\GitHub\CienciasNaturales\fuentes\contenidos\grado07\guion07\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\German\Documents\Aulaplaneta All\Trabajos de editor\EDITOR\ESCALETAS\Escaletas  grupo  3\CN_07_07_CO\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -686,9 +686,6 @@
     <t>Recurso M5D-02</t>
   </si>
   <si>
-    <t>Tipos de energía y sus transformaciones</t>
-  </si>
-  <si>
     <t>Flujos de energía en los ecosistemas</t>
   </si>
   <si>
@@ -750,13 +747,16 @@
   </si>
   <si>
     <t>Interactivo en el que se explica, con dos ejemplos, cómo se clasifican los ciclos biogeoquímicos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Las formas de la energía y sus transformaciones </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -765,6 +765,14 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -802,6 +810,20 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="3"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -935,20 +957,20 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="97">
+  <cellXfs count="99">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -956,27 +978,27 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -992,22 +1014,22 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1017,50 +1039,98 @@
     <xf numFmtId="0" fontId="1" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="1" xfId="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="1" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1074,7 +1144,7 @@
     <xf numFmtId="0" fontId="1" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1087,48 +1157,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1438,8 +1466,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U298"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="L52" sqref="L52"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="C50" sqref="A1:XFD50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1468,101 +1496,101 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" s="9" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="85" t="s">
+      <c r="A1" s="78" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="87" t="s">
+      <c r="B1" s="80" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="89" t="s">
+      <c r="C1" s="82" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="85" t="s">
+      <c r="D1" s="78" t="s">
         <v>111</v>
       </c>
-      <c r="E1" s="87" t="s">
+      <c r="E1" s="80" t="s">
         <v>112</v>
       </c>
-      <c r="F1" s="91" t="s">
+      <c r="F1" s="84" t="s">
         <v>113</v>
       </c>
-      <c r="G1" s="83" t="s">
+      <c r="G1" s="76" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="91" t="s">
+      <c r="H1" s="84" t="s">
         <v>114</v>
       </c>
-      <c r="I1" s="91" t="s">
+      <c r="I1" s="84" t="s">
         <v>108</v>
       </c>
-      <c r="J1" s="93" t="s">
+      <c r="J1" s="86" t="s">
         <v>4</v>
       </c>
-      <c r="K1" s="95" t="s">
+      <c r="K1" s="88" t="s">
         <v>109</v>
       </c>
-      <c r="L1" s="83" t="s">
+      <c r="L1" s="76" t="s">
         <v>14</v>
       </c>
-      <c r="M1" s="78" t="s">
+      <c r="M1" s="94" t="s">
         <v>21</v>
       </c>
-      <c r="N1" s="78"/>
-      <c r="O1" s="79" t="s">
+      <c r="N1" s="94"/>
+      <c r="O1" s="95" t="s">
         <v>110</v>
       </c>
-      <c r="P1" s="79" t="s">
+      <c r="P1" s="95" t="s">
         <v>115</v>
       </c>
-      <c r="Q1" s="76" t="s">
+      <c r="Q1" s="92" t="s">
         <v>86</v>
       </c>
-      <c r="R1" s="81" t="s">
+      <c r="R1" s="97" t="s">
         <v>87</v>
       </c>
-      <c r="S1" s="76" t="s">
+      <c r="S1" s="92" t="s">
         <v>88</v>
       </c>
-      <c r="T1" s="74" t="s">
+      <c r="T1" s="90" t="s">
         <v>89</v>
       </c>
-      <c r="U1" s="76" t="s">
+      <c r="U1" s="92" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="2" spans="1:21" s="9" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="86"/>
-      <c r="B2" s="88"/>
-      <c r="C2" s="90"/>
-      <c r="D2" s="86"/>
-      <c r="E2" s="88"/>
-      <c r="F2" s="92"/>
-      <c r="G2" s="84"/>
-      <c r="H2" s="92"/>
-      <c r="I2" s="92"/>
-      <c r="J2" s="94"/>
-      <c r="K2" s="96"/>
-      <c r="L2" s="84"/>
+      <c r="A2" s="79"/>
+      <c r="B2" s="81"/>
+      <c r="C2" s="83"/>
+      <c r="D2" s="79"/>
+      <c r="E2" s="81"/>
+      <c r="F2" s="85"/>
+      <c r="G2" s="77"/>
+      <c r="H2" s="85"/>
+      <c r="I2" s="85"/>
+      <c r="J2" s="87"/>
+      <c r="K2" s="89"/>
+      <c r="L2" s="77"/>
       <c r="M2" s="10" t="s">
         <v>91</v>
       </c>
       <c r="N2" s="10" t="s">
         <v>92</v>
       </c>
-      <c r="O2" s="80"/>
-      <c r="P2" s="80"/>
-      <c r="Q2" s="77"/>
-      <c r="R2" s="82"/>
-      <c r="S2" s="77"/>
-      <c r="T2" s="75"/>
-      <c r="U2" s="77"/>
+      <c r="O2" s="96"/>
+      <c r="P2" s="96"/>
+      <c r="Q2" s="93"/>
+      <c r="R2" s="98"/>
+      <c r="S2" s="93"/>
+      <c r="T2" s="91"/>
+      <c r="U2" s="93"/>
     </row>
     <row r="3" spans="1:21" s="35" customFormat="1" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A3" s="11" t="s">
         <v>122</v>
       </c>
       <c r="B3" s="34" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>123</v>
@@ -1571,7 +1599,7 @@
         <v>124</v>
       </c>
       <c r="E3" s="6"/>
-      <c r="F3" s="72"/>
+      <c r="F3" s="73"/>
       <c r="G3" s="38"/>
       <c r="H3" s="25"/>
       <c r="I3" s="16"/>
@@ -1582,18 +1610,18 @@
       <c r="N3" s="20"/>
       <c r="O3" s="8"/>
       <c r="P3" s="25"/>
-      <c r="Q3" s="69"/>
-      <c r="R3" s="70"/>
-      <c r="S3" s="69"/>
-      <c r="T3" s="71"/>
-      <c r="U3" s="69"/>
+      <c r="Q3" s="70"/>
+      <c r="R3" s="71"/>
+      <c r="S3" s="70"/>
+      <c r="T3" s="72"/>
+      <c r="U3" s="70"/>
     </row>
     <row r="4" spans="1:21" s="35" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="11" t="s">
         <v>122</v>
       </c>
       <c r="B4" s="34" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>123</v>
@@ -1604,7 +1632,7 @@
       <c r="E4" s="6" t="s">
         <v>125</v>
       </c>
-      <c r="F4" s="72"/>
+      <c r="F4" s="73"/>
       <c r="G4" s="38"/>
       <c r="H4" s="25"/>
       <c r="I4" s="16"/>
@@ -1615,18 +1643,18 @@
       <c r="N4" s="20"/>
       <c r="O4" s="8"/>
       <c r="P4" s="25"/>
-      <c r="Q4" s="69"/>
-      <c r="R4" s="70"/>
-      <c r="S4" s="69"/>
-      <c r="T4" s="71"/>
-      <c r="U4" s="69"/>
+      <c r="Q4" s="70"/>
+      <c r="R4" s="71"/>
+      <c r="S4" s="70"/>
+      <c r="T4" s="72"/>
+      <c r="U4" s="70"/>
     </row>
     <row r="5" spans="1:21" s="35" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="11" t="s">
         <v>122</v>
       </c>
       <c r="B5" s="34" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>123</v>
@@ -1637,8 +1665,8 @@
       <c r="E5" s="6" t="s">
         <v>125</v>
       </c>
-      <c r="F5" s="73" t="s">
-        <v>220</v>
+      <c r="F5" s="75" t="s">
+        <v>241</v>
       </c>
       <c r="G5" s="38" t="s">
         <v>130</v>
@@ -1666,19 +1694,19 @@
       <c r="P5" s="25" t="s">
         <v>19</v>
       </c>
-      <c r="Q5" s="69">
+      <c r="Q5" s="70">
         <v>6</v>
       </c>
-      <c r="R5" s="70" t="s">
+      <c r="R5" s="71" t="s">
         <v>194</v>
       </c>
-      <c r="S5" s="69" t="s">
+      <c r="S5" s="70" t="s">
         <v>195</v>
       </c>
-      <c r="T5" s="71" t="s">
+      <c r="T5" s="72" t="s">
         <v>199</v>
       </c>
-      <c r="U5" s="69" t="s">
+      <c r="U5" s="70" t="s">
         <v>196</v>
       </c>
     </row>
@@ -1687,7 +1715,7 @@
         <v>122</v>
       </c>
       <c r="B6" s="54" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C6" s="55" t="s">
         <v>123</v>
@@ -1711,7 +1739,7 @@
         <v>20</v>
       </c>
       <c r="J6" s="60" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="K6" s="61" t="s">
         <v>20</v>
@@ -1748,7 +1776,7 @@
         <v>122</v>
       </c>
       <c r="B7" s="43" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C7" s="44" t="s">
         <v>123</v>
@@ -1807,7 +1835,7 @@
         <v>122</v>
       </c>
       <c r="B8" s="34" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C8" s="36" t="s">
         <v>123</v>
@@ -1838,7 +1866,7 @@
         <v>122</v>
       </c>
       <c r="B9" s="34" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C9" s="36" t="s">
         <v>123</v>
@@ -1871,7 +1899,7 @@
         <v>122</v>
       </c>
       <c r="B10" s="34" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C10" s="33" t="s">
         <v>123</v>
@@ -1930,7 +1958,7 @@
         <v>122</v>
       </c>
       <c r="B11" s="43" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C11" s="44" t="s">
         <v>123</v>
@@ -1989,13 +2017,13 @@
         <v>122</v>
       </c>
       <c r="B12" s="34" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C12" s="36" t="s">
         <v>123</v>
       </c>
       <c r="D12" s="37" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="E12" s="34"/>
       <c r="F12" s="8"/>
@@ -2020,13 +2048,13 @@
         <v>122</v>
       </c>
       <c r="B13" s="34" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C13" s="36" t="s">
         <v>123</v>
       </c>
       <c r="D13" s="37" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="E13" s="34" t="s">
         <v>133</v>
@@ -2053,13 +2081,13 @@
         <v>122</v>
       </c>
       <c r="B14" s="34" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C14" s="36" t="s">
         <v>123</v>
       </c>
       <c r="D14" s="37" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="E14" s="34" t="s">
         <v>135</v>
@@ -2086,13 +2114,13 @@
         <v>122</v>
       </c>
       <c r="B15" s="34" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C15" s="36" t="s">
         <v>123</v>
       </c>
       <c r="D15" s="37" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="E15" s="34" t="s">
         <v>135</v>
@@ -2121,13 +2149,13 @@
         <v>122</v>
       </c>
       <c r="B16" s="34" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C16" s="36" t="s">
         <v>123</v>
       </c>
       <c r="D16" s="37" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="E16" s="34" t="s">
         <v>135</v>
@@ -2145,7 +2173,7 @@
         <v>20</v>
       </c>
       <c r="J16" s="60" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="K16" s="61" t="s">
         <v>20</v>
@@ -2158,7 +2186,7 @@
         <v>120</v>
       </c>
       <c r="O16" s="8"/>
-      <c r="P16" s="25" t="s">
+      <c r="P16" s="69" t="s">
         <v>20</v>
       </c>
       <c r="Q16" s="64">
@@ -2182,13 +2210,13 @@
         <v>122</v>
       </c>
       <c r="B17" s="34" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C17" s="36" t="s">
         <v>123</v>
       </c>
       <c r="D17" s="37" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="E17" s="34" t="s">
         <v>135</v>
@@ -2222,19 +2250,19 @@
       <c r="P17" s="25" t="s">
         <v>19</v>
       </c>
-      <c r="Q17" s="69">
+      <c r="Q17" s="70">
         <v>6</v>
       </c>
-      <c r="R17" s="70" t="s">
+      <c r="R17" s="71" t="s">
         <v>194</v>
       </c>
-      <c r="S17" s="69" t="s">
+      <c r="S17" s="70" t="s">
         <v>195</v>
       </c>
-      <c r="T17" s="71" t="s">
+      <c r="T17" s="72" t="s">
         <v>200</v>
       </c>
-      <c r="U17" s="69" t="s">
+      <c r="U17" s="70" t="s">
         <v>196</v>
       </c>
     </row>
@@ -2243,13 +2271,13 @@
         <v>122</v>
       </c>
       <c r="B18" s="34" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C18" s="36" t="s">
         <v>123</v>
       </c>
       <c r="D18" s="37" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="E18" s="34" t="s">
         <v>135</v>
@@ -2304,13 +2332,13 @@
         <v>122</v>
       </c>
       <c r="B19" s="43" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C19" s="44" t="s">
         <v>123</v>
       </c>
       <c r="D19" s="37" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="E19" s="43" t="s">
         <v>132</v>
@@ -2363,7 +2391,7 @@
         <v>122</v>
       </c>
       <c r="B20" s="34" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C20" s="36" t="s">
         <v>123</v>
@@ -2394,7 +2422,7 @@
         <v>122</v>
       </c>
       <c r="B21" s="34" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C21" s="36" t="s">
         <v>123</v>
@@ -2453,7 +2481,7 @@
         <v>122</v>
       </c>
       <c r="B22" s="54" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C22" s="55" t="s">
         <v>123</v>
@@ -2475,18 +2503,18 @@
       <c r="N22" s="63"/>
       <c r="O22" s="57"/>
       <c r="P22" s="25"/>
-      <c r="Q22" s="69"/>
-      <c r="R22" s="70"/>
-      <c r="S22" s="69"/>
-      <c r="T22" s="71"/>
-      <c r="U22" s="69"/>
+      <c r="Q22" s="70"/>
+      <c r="R22" s="71"/>
+      <c r="S22" s="70"/>
+      <c r="T22" s="72"/>
+      <c r="U22" s="70"/>
     </row>
     <row r="23" spans="1:21" s="67" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A23" s="53" t="s">
         <v>122</v>
       </c>
       <c r="B23" s="54" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C23" s="55" t="s">
         <v>123</v>
@@ -2510,7 +2538,7 @@
         <v>19</v>
       </c>
       <c r="J23" s="60" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="K23" s="61" t="s">
         <v>20</v>
@@ -2526,19 +2554,19 @@
       <c r="P23" s="25" t="s">
         <v>19</v>
       </c>
-      <c r="Q23" s="69">
+      <c r="Q23" s="70">
         <v>6</v>
       </c>
-      <c r="R23" s="70" t="s">
+      <c r="R23" s="71" t="s">
         <v>194</v>
       </c>
-      <c r="S23" s="69" t="s">
+      <c r="S23" s="70" t="s">
         <v>195</v>
       </c>
-      <c r="T23" s="71" t="s">
+      <c r="T23" s="72" t="s">
         <v>201</v>
       </c>
-      <c r="U23" s="69" t="s">
+      <c r="U23" s="70" t="s">
         <v>196</v>
       </c>
     </row>
@@ -2547,7 +2575,7 @@
         <v>122</v>
       </c>
       <c r="B24" s="43" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C24" s="44" t="s">
         <v>123</v>
@@ -2606,7 +2634,7 @@
         <v>122</v>
       </c>
       <c r="B25" s="34" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C25" s="36" t="s">
         <v>123</v>
@@ -2637,7 +2665,7 @@
         <v>122</v>
       </c>
       <c r="B26" s="34" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C26" s="36" t="s">
         <v>123</v>
@@ -2670,7 +2698,7 @@
         <v>122</v>
       </c>
       <c r="B27" s="34" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C27" s="36" t="s">
         <v>123</v>
@@ -2705,7 +2733,7 @@
         <v>122</v>
       </c>
       <c r="B28" s="34" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C28" s="36" t="s">
         <v>123</v>
@@ -2729,7 +2757,7 @@
         <v>20</v>
       </c>
       <c r="J28" s="39" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="K28" s="18" t="s">
         <v>20</v>
@@ -2766,7 +2794,7 @@
         <v>122</v>
       </c>
       <c r="B29" s="34" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C29" s="36" t="s">
         <v>123</v>
@@ -2799,7 +2827,7 @@
         <v>122</v>
       </c>
       <c r="B30" s="34" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C30" s="36" t="s">
         <v>123</v>
@@ -2834,7 +2862,7 @@
         <v>122</v>
       </c>
       <c r="B31" s="34" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C31" s="36" t="s">
         <v>123</v>
@@ -2858,7 +2886,7 @@
         <v>20</v>
       </c>
       <c r="J31" s="39" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="K31" s="18" t="s">
         <v>20</v>
@@ -2871,7 +2899,7 @@
         <v>121</v>
       </c>
       <c r="O31" s="8"/>
-      <c r="P31" s="25" t="s">
+      <c r="P31" s="69" t="s">
         <v>20</v>
       </c>
       <c r="Q31" s="64">
@@ -2895,7 +2923,7 @@
         <v>122</v>
       </c>
       <c r="B32" s="34" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C32" s="36" t="s">
         <v>123</v>
@@ -2916,7 +2944,7 @@
       <c r="M32" s="20"/>
       <c r="N32" s="20"/>
       <c r="O32" s="8"/>
-      <c r="P32" s="25"/>
+      <c r="P32" s="69"/>
       <c r="Q32" s="64"/>
       <c r="R32" s="65"/>
       <c r="S32" s="64"/>
@@ -2928,7 +2956,7 @@
         <v>122</v>
       </c>
       <c r="B33" s="34" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C33" s="36" t="s">
         <v>123</v>
@@ -2963,7 +2991,7 @@
         <v>122</v>
       </c>
       <c r="B34" s="34" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C34" s="36" t="s">
         <v>123</v>
@@ -2987,7 +3015,7 @@
         <v>20</v>
       </c>
       <c r="J34" s="39" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="K34" s="18" t="s">
         <v>20</v>
@@ -3013,7 +3041,7 @@
         <v>203</v>
       </c>
       <c r="T34" s="66" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="U34" s="64" t="s">
         <v>205</v>
@@ -3024,7 +3052,7 @@
         <v>122</v>
       </c>
       <c r="B35" s="34" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C35" s="36" t="s">
         <v>123</v>
@@ -3057,7 +3085,7 @@
         <v>122</v>
       </c>
       <c r="B36" s="34" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C36" s="36" t="s">
         <v>123</v>
@@ -3092,7 +3120,7 @@
         <v>122</v>
       </c>
       <c r="B37" s="34" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C37" s="36" t="s">
         <v>123</v>
@@ -3116,7 +3144,7 @@
         <v>20</v>
       </c>
       <c r="J37" s="39" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="K37" s="18" t="s">
         <v>20</v>
@@ -3129,7 +3157,7 @@
         <v>36</v>
       </c>
       <c r="O37" s="8"/>
-      <c r="P37" s="25" t="s">
+      <c r="P37" s="69" t="s">
         <v>20</v>
       </c>
       <c r="Q37" s="64">
@@ -3153,7 +3181,7 @@
         <v>122</v>
       </c>
       <c r="B38" s="34" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C38" s="36" t="s">
         <v>123</v>
@@ -3168,7 +3196,7 @@
         <v>159</v>
       </c>
       <c r="G38" s="38" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="H38" s="25">
         <v>17</v>
@@ -3177,7 +3205,7 @@
         <v>19</v>
       </c>
       <c r="J38" s="39" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="K38" s="18" t="s">
         <v>20</v>
@@ -3214,7 +3242,7 @@
         <v>122</v>
       </c>
       <c r="B39" s="34" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C39" s="36" t="s">
         <v>123</v>
@@ -3238,7 +3266,7 @@
         <v>20</v>
       </c>
       <c r="J39" s="39" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="K39" s="18" t="s">
         <v>20</v>
@@ -3264,7 +3292,7 @@
         <v>203</v>
       </c>
       <c r="T39" s="66" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="U39" s="64" t="s">
         <v>205</v>
@@ -3275,7 +3303,7 @@
         <v>122</v>
       </c>
       <c r="B40" s="54" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C40" s="55" t="s">
         <v>123</v>
@@ -3299,7 +3327,7 @@
         <v>20</v>
       </c>
       <c r="J40" s="60" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="K40" s="61" t="s">
         <v>20</v>
@@ -3312,7 +3340,7 @@
         <v>32</v>
       </c>
       <c r="O40" s="57"/>
-      <c r="P40" s="59" t="s">
+      <c r="P40" s="74" t="s">
         <v>20</v>
       </c>
       <c r="Q40" s="64">
@@ -3336,7 +3364,7 @@
         <v>122</v>
       </c>
       <c r="B41" s="43" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C41" s="44" t="s">
         <v>123</v>
@@ -3395,7 +3423,7 @@
         <v>122</v>
       </c>
       <c r="B42" s="34" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C42" s="36" t="s">
         <v>123</v>
@@ -3441,7 +3469,7 @@
         <v>195</v>
       </c>
       <c r="T42" s="66" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="U42" s="64" t="s">
         <v>196</v>
@@ -3452,7 +3480,7 @@
         <v>122</v>
       </c>
       <c r="B43" s="34" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C43" s="36" t="s">
         <v>123</v>
@@ -3485,7 +3513,7 @@
       </c>
       <c r="N43" s="20"/>
       <c r="O43" s="8"/>
-      <c r="P43" s="25" t="s">
+      <c r="P43" s="69" t="s">
         <v>20</v>
       </c>
       <c r="Q43" s="64">
@@ -3498,7 +3526,7 @@
         <v>195</v>
       </c>
       <c r="T43" s="66" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="U43" s="64" t="s">
         <v>196</v>
@@ -3509,7 +3537,7 @@
         <v>122</v>
       </c>
       <c r="B44" s="34" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C44" s="36" t="s">
         <v>123</v>
@@ -3555,7 +3583,7 @@
         <v>203</v>
       </c>
       <c r="T44" s="66" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="U44" s="64" t="s">
         <v>205</v>
@@ -3566,7 +3594,7 @@
         <v>122</v>
       </c>
       <c r="B45" s="34" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C45" s="36" t="s">
         <v>123</v>
@@ -3586,7 +3614,7 @@
         <v>20</v>
       </c>
       <c r="J45" s="39" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="K45" s="18" t="s">
         <v>20</v>
@@ -3609,7 +3637,7 @@
         <v>122</v>
       </c>
       <c r="B46" s="34" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C46" s="36" t="s">
         <v>123</v>
@@ -3629,7 +3657,7 @@
         <v>20</v>
       </c>
       <c r="J46" s="39" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="K46" s="18" t="s">
         <v>20</v>
@@ -3666,7 +3694,7 @@
         <v>122</v>
       </c>
       <c r="B47" s="34" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C47" s="36" t="s">
         <v>123</v>
@@ -3686,7 +3714,7 @@
         <v>20</v>
       </c>
       <c r="J47" s="39" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="K47" s="18" t="s">
         <v>20</v>
@@ -3700,7 +3728,7 @@
       </c>
       <c r="O47" s="8"/>
       <c r="P47" s="25" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="Q47" s="64">
         <v>6</v>
@@ -4932,6 +4960,14 @@
     <row r="298" hidden="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="T1:T2"/>
+    <mergeCell ref="U1:U2"/>
+    <mergeCell ref="M1:N1"/>
+    <mergeCell ref="O1:O2"/>
+    <mergeCell ref="P1:P2"/>
+    <mergeCell ref="Q1:Q2"/>
+    <mergeCell ref="R1:R2"/>
+    <mergeCell ref="S1:S2"/>
     <mergeCell ref="L1:L2"/>
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="B1:B2"/>
@@ -4944,14 +4980,6 @@
     <mergeCell ref="I1:I2"/>
     <mergeCell ref="J1:J2"/>
     <mergeCell ref="K1:K2"/>
-    <mergeCell ref="T1:T2"/>
-    <mergeCell ref="U1:U2"/>
-    <mergeCell ref="M1:N1"/>
-    <mergeCell ref="O1:O2"/>
-    <mergeCell ref="P1:P2"/>
-    <mergeCell ref="Q1:Q2"/>
-    <mergeCell ref="R1:R2"/>
-    <mergeCell ref="S1:S2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>